<commit_message>
Added a transistor to the LCD backlight so it can be controlled by the Teensy.  Also added a jumper so it can be turned on manually.  Updated the BOM.
</commit_message>
<xml_diff>
--- a/internal_env_board/internal_env_board2/internal_env_board_with_LCD_BOM.xlsx
+++ b/internal_env_board/internal_env_board2/internal_env_board_with_LCD_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARVP\au_hardware\internal_env_board\internal_env_board2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boyle\Documents\AVRP repository\au_hardware\internal_env_board\internal_env_board2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C6BB1A-7FB6-4551-891D-32C787919B87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44844C58-25A9-459B-80F8-58306FFE1E8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -312,30 +312,12 @@
     <t>C6</t>
   </si>
   <si>
-    <t>8 bit shift register - DIP package</t>
-  </si>
-  <si>
-    <t>560 Ohm Resistor</t>
-  </si>
-  <si>
-    <t>0.1 uF cap</t>
-  </si>
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
     <t>74HC595D,118</t>
   </si>
   <si>
     <t>https://assets.nexperia.com/documents/data-sheet/74HC_HCT595.pdf</t>
   </si>
   <si>
-    <t>ERJ-PB6D5600V</t>
-  </si>
-  <si>
-    <t>ERJ-PB3, PB6 Series, High Precision Datasheet</t>
-  </si>
-  <si>
     <t>CL21F104ZBCNNNC</t>
   </si>
   <si>
@@ -345,12 +327,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>16x2 LCD</t>
-  </si>
-  <si>
-    <t>https://cdn-shop.adafruit.com/datasheets/HD44780.pdf , https://cdn-shop.adafruit.com/product-files/181/p181.pdf</t>
-  </si>
-  <si>
     <t>6130xx11121 Drawing</t>
   </si>
   <si>
@@ -369,24 +345,12 @@
     <t>K104K10X7RF5UH5</t>
   </si>
   <si>
-    <t xml:space="preserve">JP5 </t>
-  </si>
-  <si>
-    <t>Ribbon Cable</t>
-  </si>
-  <si>
     <t>111-2413-020</t>
   </si>
   <si>
-    <t>Ribbon Cable Connector</t>
-  </si>
-  <si>
     <t>4-643814-6</t>
   </si>
   <si>
-    <t>Connector Stress Strain Relief</t>
-  </si>
-  <si>
     <t>1-643075-6</t>
   </si>
   <si>
@@ -402,17 +366,134 @@
     <t>N/A (LCDs)</t>
   </si>
   <si>
-    <t>https://cdn-shop.adafruit.com/product-files/181/p181.pdf</t>
-  </si>
-  <si>
-    <t>10k Potentiometer (comes with the LCDs)</t>
+    <t>SM-42TA203</t>
+  </si>
+  <si>
+    <t>SM-42 &amp; 43 Series Datasheet</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>JP6</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>TRANS NPN 40V 0.2A SOT23</t>
+  </si>
+  <si>
+    <t>MMBT3904</t>
+  </si>
+  <si>
+    <t>2N3904, MMBT3904, PZT3904 Datasheet</t>
+  </si>
+  <si>
+    <t>02+02 DIL VERT PIN HDR</t>
+  </si>
+  <si>
+    <t>M20-9760246</t>
+  </si>
+  <si>
+    <t>M20-976yyyy Drawing</t>
+  </si>
+  <si>
+    <t>RES SMD 47K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805FR-0747KL</t>
+  </si>
+  <si>
+    <t>RC Series, L Datasheet</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805JR-074K7L</t>
+  </si>
+  <si>
+    <t>TC1602A-09T</t>
+  </si>
+  <si>
+    <t>TRANS NPN 40V 0.2A TO-92</t>
+  </si>
+  <si>
+    <t>2N3904BU</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1/4W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>CF14JT4K70</t>
+  </si>
+  <si>
+    <t>CF, CFM Series</t>
+  </si>
+  <si>
+    <t>RES 47K OHM 1/4W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>CF14JT47K0</t>
+  </si>
+  <si>
+    <t>IC SHIFT REGISTER 8BIT 16SOIC</t>
+  </si>
+  <si>
+    <t>RES SMD 560 OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC0805JR-07560RL</t>
+  </si>
+  <si>
+    <t>TRIMMER 20KOHM 0.25W J LEAD SIDE</t>
+  </si>
+  <si>
+    <t>CONN HEADER 16 POS 2.54</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V Y5V 0805</t>
+  </si>
+  <si>
+    <t>STANDARD LCD 16X2 + EXTRAS</t>
+  </si>
+  <si>
+    <t>IC 8-BIT SHIFT REGISTER 16-DIP</t>
+  </si>
+  <si>
+    <t>RES 560 OHM 1/4W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R RADIAL</t>
+  </si>
+  <si>
+    <t>CBL RIBN 20COND MULTICOLOR 5'</t>
+  </si>
+  <si>
+    <t>CONN RECEPT 16POS 24AWG MTA100</t>
+  </si>
+  <si>
+    <t>CONN COVER STRAIN RELIEF 16 POS</t>
+  </si>
+  <si>
+    <t>3362P-1-203LF</t>
+  </si>
+  <si>
+    <t>3362 Series</t>
+  </si>
+  <si>
+    <t>TRIMMER 20K OHM 0.5W PC PIN TOP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,17 +516,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -456,7 +531,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -479,12 +554,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -496,25 +595,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -523,15 +609,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -813,32 +919,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,7 +967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -885,7 +991,7 @@
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>73</v>
       </c>
@@ -909,7 +1015,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -933,7 +1039,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -957,7 +1063,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -981,7 +1087,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>64</v>
       </c>
@@ -1005,7 +1111,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
@@ -1029,7 +1135,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -1053,14 +1159,14 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="9">
         <v>39281023</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1077,7 +1183,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1101,7 +1207,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
@@ -1125,7 +1231,7 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -1149,7 +1255,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -1173,7 +1279,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -1197,7 +1303,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -1221,7 +1327,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1245,7 +1351,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>68</v>
       </c>
@@ -1269,7 +1375,7 @@
         <v>14.73</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -1293,7 +1399,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -1317,7 +1423,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -1341,7 +1447,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>77</v>
       </c>
@@ -1365,7 +1471,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>84</v>
       </c>
@@ -1389,317 +1495,469 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="8">
+      <c r="D25" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="6">
         <v>0.65</v>
       </c>
-      <c r="F25" s="8">
-        <v>1</v>
-      </c>
-      <c r="G25" s="8">
+      <c r="F25" s="6">
+        <v>1</v>
+      </c>
+      <c r="G25" s="6">
         <v>0.65</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>94</v>
+      <c r="B26" s="15" t="s">
+        <v>137</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="F26" s="8">
+        <v>138</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="F26" s="6">
         <v>6</v>
       </c>
-      <c r="G26" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="G26" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="4">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="6">
+        <v>5.2</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="16">
+      <c r="B28" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="11">
         <v>61301611121</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="12">
+      <c r="D28" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="6">
         <v>1.29</v>
       </c>
-      <c r="F28" s="12">
-        <v>1</v>
-      </c>
-      <c r="G28" s="12">
+      <c r="F28" s="6">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6">
         <v>1.29</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="D29" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F29" s="6">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="19">
+        <v>181</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="6">
+        <v>14.28</v>
+      </c>
+      <c r="F30" s="6">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6">
+        <v>14.28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="F31" s="16">
+        <v>1</v>
+      </c>
+      <c r="G31" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="F32" s="16">
+        <v>1</v>
+      </c>
+      <c r="G32" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0.27</v>
+      </c>
+      <c r="F33" s="16">
+        <v>1</v>
+      </c>
+      <c r="G33" s="16">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F34" s="16">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="F38" s="6">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="B39" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E29" s="8">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F29" s="8">
-        <v>1</v>
-      </c>
-      <c r="G29" s="8">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="D39" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="F39" s="6">
+        <v>6</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="F40" s="6">
+        <v>1</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="17">
-        <v>181</v>
-      </c>
-      <c r="D30" s="9" t="s">
+      <c r="D41" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="6">
+        <v>22.01</v>
+      </c>
+      <c r="F41" s="6">
+        <v>1</v>
+      </c>
+      <c r="G41" s="6">
+        <v>22.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="8">
-        <v>14.28</v>
-      </c>
-      <c r="F30" s="8">
-        <v>1</v>
-      </c>
-      <c r="G30" s="8">
-        <v>14.28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="D42" s="7">
+        <v>643814</v>
+      </c>
+      <c r="E42" s="6">
+        <v>4.54</v>
+      </c>
+      <c r="F42" s="6">
+        <v>2</v>
+      </c>
+      <c r="G42" s="6">
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="7">
+        <v>643075</v>
+      </c>
+      <c r="E43" s="6">
+        <v>1.31</v>
+      </c>
+      <c r="F43" s="6">
+        <v>2</v>
+      </c>
+      <c r="G43" s="6">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="F44" s="16">
+        <v>1</v>
+      </c>
+      <c r="G44" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="F45" s="16">
+        <v>1</v>
+      </c>
+      <c r="G45" s="16">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E33" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F33" s="8">
-        <v>1</v>
-      </c>
-      <c r="G33" s="8">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E34" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F34" s="8">
-        <v>6</v>
-      </c>
-      <c r="G34" s="8">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="8">
-        <v>0.33</v>
-      </c>
-      <c r="F35" s="8">
-        <v>1</v>
-      </c>
-      <c r="G35" s="8">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="18">
-        <v>61301611121</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="8">
-        <v>1.29</v>
-      </c>
-      <c r="F37" s="8">
-        <v>1</v>
-      </c>
-      <c r="G37" s="8">
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" s="8">
-        <v>22.01</v>
-      </c>
-      <c r="F38" s="8">
-        <v>1</v>
-      </c>
-      <c r="G38" s="8">
-        <v>22.01</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="10">
-        <v>643814</v>
-      </c>
-      <c r="E39" s="8">
-        <v>4.54</v>
-      </c>
-      <c r="F39" s="8">
-        <v>2</v>
-      </c>
-      <c r="G39" s="8">
-        <v>9.08</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="10">
-        <v>643075</v>
-      </c>
-      <c r="E40" s="8">
-        <v>1.31</v>
-      </c>
-      <c r="F40" s="8">
-        <v>2</v>
-      </c>
-      <c r="G40" s="8">
-        <v>2.61</v>
+      <c r="E46" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="F46" s="16">
+        <v>1</v>
+      </c>
+      <c r="G46" s="16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="6">
+        <v>1.56</v>
+      </c>
+      <c r="F47" s="6">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6">
+        <v>1.56</v>
       </c>
     </row>
   </sheetData>
@@ -1731,17 +1989,25 @@
     <hyperlink ref="D24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="D25" r:id="rId23" xr:uid="{3351DE6A-696D-4930-A7F0-EEAC89FE5E4D}"/>
     <hyperlink ref="D29" r:id="rId24" xr:uid="{484C9603-5306-41D1-80A8-846D2759712C}"/>
-    <hyperlink ref="D26" r:id="rId25" display="https://industrial.panasonic.com/cdbs/www-data/pdf/RDM0000/AOA0000C328.pdf" xr:uid="{235D67A7-AF17-49DF-8540-EC27D3B31A1D}"/>
-    <hyperlink ref="D28" r:id="rId26" display="https://katalog.we-online.de/em/datasheet/6130xx11121.pdf" xr:uid="{A4FD35A8-382F-4C86-9E06-5143FCB65F6D}"/>
-    <hyperlink ref="D33" r:id="rId27" display="http://www.ti.com/lit/ds/symlink/sn74hc595.pdf" xr:uid="{06113F77-C44E-4230-9895-41937B419CB7}"/>
-    <hyperlink ref="D35" r:id="rId28" display="http://www.vishay.com/docs/45171/kseries.pdf" xr:uid="{E5EF8C94-8FF3-4CA8-9B9E-87F6E9DB4092}"/>
-    <hyperlink ref="D34" r:id="rId29" xr:uid="{FC8D83A5-9C1A-4F8F-B14D-32D28D960C5F}"/>
-    <hyperlink ref="D37" r:id="rId30" display="https://katalog.we-online.de/em/datasheet/6130xx11121.pdf" xr:uid="{A4FD35A8-382F-4C86-9E06-5143FCB65F6D}"/>
-    <hyperlink ref="D39" r:id="rId31" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643814&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{E3A30A47-2BA3-4731-BBCD-B356DAFFADB8}"/>
-    <hyperlink ref="D40" r:id="rId32" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643075&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{8B16C1D1-DD20-434B-8323-AF5F2EDA724D}"/>
-    <hyperlink ref="D27" r:id="rId33" xr:uid="{539E45F2-FB86-48A2-A893-55EE399073A4}"/>
+    <hyperlink ref="D28" r:id="rId25" display="https://katalog.we-online.de/em/datasheet/6130xx11121.pdf" xr:uid="{A4FD35A8-382F-4C86-9E06-5143FCB65F6D}"/>
+    <hyperlink ref="D38" r:id="rId26" display="http://www.ti.com/lit/ds/symlink/sn74hc595.pdf" xr:uid="{06113F77-C44E-4230-9895-41937B419CB7}"/>
+    <hyperlink ref="D40" r:id="rId27" display="http://www.vishay.com/docs/45171/kseries.pdf" xr:uid="{E5EF8C94-8FF3-4CA8-9B9E-87F6E9DB4092}"/>
+    <hyperlink ref="D39" r:id="rId28" xr:uid="{FC8D83A5-9C1A-4F8F-B14D-32D28D960C5F}"/>
+    <hyperlink ref="D42" r:id="rId29" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643814&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{E3A30A47-2BA3-4731-BBCD-B356DAFFADB8}"/>
+    <hyperlink ref="D43" r:id="rId30" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643075&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{8B16C1D1-DD20-434B-8323-AF5F2EDA724D}"/>
+    <hyperlink ref="D27" r:id="rId31" display="https://www.nidec-copal-electronics.com/e/catalog/trimmer/sm-42&amp;sm-43.pdf" xr:uid="{D60C1852-FE22-4206-B3C9-619A0EF72358}"/>
+    <hyperlink ref="D34" r:id="rId32" display="https://www.onsemi.com/pub/Collateral/PZT3904-D.pdf" xr:uid="{9523DBC2-EEE9-478C-ADAF-70DD47AC3E92}"/>
+    <hyperlink ref="D33" r:id="rId33" display="https://cdn.harwin.com/pdfs/M20-976.pdf" xr:uid="{34521EE4-CF7E-4C34-8BD1-8EFE6C6D15C2}"/>
+    <hyperlink ref="D32" r:id="rId34" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf" xr:uid="{B2D11C3C-0234-4231-ABA9-DAD532102B77}"/>
+    <hyperlink ref="D31" r:id="rId35" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf" xr:uid="{31B22529-345B-4FCB-8E6C-90977DD52DC7}"/>
+    <hyperlink ref="D30" r:id="rId36" display="https://cdn-shop.adafruit.com/product-files/181/p181.pdf" xr:uid="{7C648116-FDBE-4031-A56C-760A7B342F84}"/>
+    <hyperlink ref="D46" r:id="rId37" display="https://www.onsemi.com/pub/Collateral/PZT3904-D.pdf" xr:uid="{522BDBC1-95E2-4FE2-8E78-6926BF8F4AB5}"/>
+    <hyperlink ref="D44" r:id="rId38" display="https://www.seielect.com/Catalog/SEI-CF_CFM.pdf" xr:uid="{B853B86B-D505-494B-B1DA-2C9007C74A6B}"/>
+    <hyperlink ref="D45" r:id="rId39" display="https://www.seielect.com/Catalog/SEI-CF_CFM.pdf" xr:uid="{D72F90B3-B09E-4086-903B-D01CF76A5649}"/>
+    <hyperlink ref="D26" r:id="rId40" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf" xr:uid="{5A507544-7488-44B1-950F-17D15B2ACC05}"/>
+    <hyperlink ref="D47" r:id="rId41" display="https://www.bourns.com/docs/Product-Datasheets/3362.pdf" xr:uid="{5D4ECA67-0725-426A-95DE-6F19F5E62251}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a transistor to the LCD backlight so it can be controlled by the Teensy.  Also added a jumper so it can be turned on manually.  Updated the BOM.  Added a jumper to BOM
</commit_message>
<xml_diff>
--- a/internal_env_board/internal_env_board2/internal_env_board_with_LCD_BOM.xlsx
+++ b/internal_env_board/internal_env_board2/internal_env_board_with_LCD_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boyle\Documents\AVRP repository\au_hardware\internal_env_board\internal_env_board2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44844C58-25A9-459B-80F8-58306FFE1E8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8308D9C-3ED7-479B-A466-3711DD01D2EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="155">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -487,13 +487,22 @@
   </si>
   <si>
     <t>TRIMMER 20K OHM 0.5W PC PIN TOP</t>
+  </si>
+  <si>
+    <t>AMP SHUNT ASS'Y</t>
+  </si>
+  <si>
+    <t>1-881545-1</t>
+  </si>
+  <si>
+    <t>881545 Drawing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,6 +530,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -583,7 +598,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -612,9 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -638,6 +650,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1499,13 +1515,13 @@
       <c r="A25" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="6">
@@ -1522,13 +1538,13 @@
       <c r="A26" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>125</v>
       </c>
       <c r="E26" s="6">
@@ -1542,16 +1558,16 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="20" t="s">
         <v>112</v>
       </c>
       <c r="E27" s="6">
@@ -1568,13 +1584,13 @@
       <c r="A28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>140</v>
       </c>
       <c r="C28" s="11">
         <v>61301611121</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="21" t="s">
         <v>98</v>
       </c>
       <c r="E28" s="6">
@@ -1591,13 +1607,13 @@
       <c r="A29" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="20" t="s">
         <v>96</v>
       </c>
       <c r="E29" s="6">
@@ -1614,13 +1630,13 @@
       <c r="A30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="18">
         <v>181</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="12" t="s">
         <v>128</v>
       </c>
       <c r="E30" s="6">
@@ -1637,22 +1653,22 @@
       <c r="A31" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>127</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="15">
         <v>0.15</v>
       </c>
-      <c r="F31" s="16">
-        <v>1</v>
-      </c>
-      <c r="G31" s="16">
+      <c r="F31" s="15">
+        <v>1</v>
+      </c>
+      <c r="G31" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -1660,22 +1676,22 @@
       <c r="A32" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="16">
+      <c r="E32" s="15">
         <v>0.15</v>
       </c>
-      <c r="F32" s="16">
-        <v>1</v>
-      </c>
-      <c r="G32" s="16">
+      <c r="F32" s="15">
+        <v>1</v>
+      </c>
+      <c r="G32" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -1683,22 +1699,22 @@
       <c r="A33" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="14" t="s">
         <v>121</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="15">
         <v>0.27</v>
       </c>
-      <c r="F33" s="16">
-        <v>1</v>
-      </c>
-      <c r="G33" s="16">
+      <c r="F33" s="15">
+        <v>1</v>
+      </c>
+      <c r="G33" s="15">
         <v>0.27</v>
       </c>
     </row>
@@ -1706,10 +1722,10 @@
       <c r="A34" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="14" t="s">
         <v>118</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -1718,7 +1734,7 @@
       <c r="E34" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="15">
         <v>1</v>
       </c>
       <c r="G34" s="1">
@@ -1734,7 +1750,7 @@
       <c r="A38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="22" t="s">
         <v>143</v>
       </c>
       <c r="C38" s="10" t="s">
@@ -1757,7 +1773,7 @@
       <c r="A39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="22" t="s">
         <v>144</v>
       </c>
       <c r="C39" s="10" t="s">
@@ -1780,7 +1796,7 @@
       <c r="A40" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="22" t="s">
         <v>145</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -1803,7 +1819,7 @@
       <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="22" t="s">
         <v>146</v>
       </c>
       <c r="C41" s="10" t="s">
@@ -1826,7 +1842,7 @@
       <c r="A42" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="22" t="s">
         <v>147</v>
       </c>
       <c r="C42" s="10" t="s">
@@ -1849,7 +1865,7 @@
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="22" t="s">
         <v>148</v>
       </c>
       <c r="C43" s="10" t="s">
@@ -1872,22 +1888,22 @@
       <c r="A44" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="14" t="s">
         <v>132</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E44" s="16">
+      <c r="E44" s="15">
         <v>0.15</v>
       </c>
-      <c r="F44" s="16">
-        <v>1</v>
-      </c>
-      <c r="G44" s="16">
+      <c r="F44" s="15">
+        <v>1</v>
+      </c>
+      <c r="G44" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -1895,22 +1911,22 @@
       <c r="A45" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="14" t="s">
         <v>135</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="16">
+      <c r="E45" s="15">
         <v>0.15</v>
       </c>
-      <c r="F45" s="16">
-        <v>1</v>
-      </c>
-      <c r="G45" s="16">
+      <c r="F45" s="15">
+        <v>1</v>
+      </c>
+      <c r="G45" s="15">
         <v>0.15</v>
       </c>
     </row>
@@ -1918,22 +1934,22 @@
       <c r="A46" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="14" t="s">
         <v>130</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E46" s="16">
+      <c r="E46" s="15">
         <v>0.3</v>
       </c>
-      <c r="F46" s="16">
-        <v>1</v>
-      </c>
-      <c r="G46" s="16">
+      <c r="F46" s="15">
+        <v>1</v>
+      </c>
+      <c r="G46" s="15">
         <v>0.3</v>
       </c>
     </row>
@@ -1941,10 +1957,10 @@
       <c r="A47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="16" t="s">
         <v>149</v>
       </c>
       <c r="D47" s="3" t="s">
@@ -1958,6 +1974,29 @@
       </c>
       <c r="G47" s="6">
         <v>1.56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E48" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="F48" s="15">
+        <v>1</v>
+      </c>
+      <c r="G48" s="15">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -2006,8 +2045,9 @@
     <hyperlink ref="D45" r:id="rId39" display="https://www.seielect.com/Catalog/SEI-CF_CFM.pdf" xr:uid="{D72F90B3-B09E-4086-903B-D01CF76A5649}"/>
     <hyperlink ref="D26" r:id="rId40" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf" xr:uid="{5A507544-7488-44B1-950F-17D15B2ACC05}"/>
     <hyperlink ref="D47" r:id="rId41" display="https://www.bourns.com/docs/Product-Datasheets/3362.pdf" xr:uid="{5D4ECA67-0725-426A-95DE-6F19F5E62251}"/>
+    <hyperlink ref="D48" r:id="rId42" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=881545&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{51B0B09B-6DDC-4FE8-A981-9C937067B97E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a new NMOS based LCD backlight control circuit to the schematic and board and add simulation files from LTspice.
</commit_message>
<xml_diff>
--- a/internal_env_board/internal_env_board2/internal_env_board_with_LCD_BOM.xlsx
+++ b/internal_env_board/internal_env_board2/internal_env_board_with_LCD_BOM.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boyle\Documents\AVRP repository\au_hardware\internal_env_board\internal_env_board2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Business\ARVP\au_hardware\internal_env_board\internal_env_board2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8308D9C-3ED7-479B-A466-3711DD01D2EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -501,7 +500,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -650,10 +649,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -934,11 +933,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,15 +949,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1741,6 +1740,12 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f>SUM(G3:G34)</f>
+        <v>58.129000000000005</v>
+      </c>
+    </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>99</v>
@@ -1980,10 +1985,10 @@
       <c r="A48" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="23" t="s">
         <v>153</v>
       </c>
       <c r="D48" s="3" t="s">
@@ -2004,48 +2009,48 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D14" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D15" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D25" r:id="rId23" xr:uid="{3351DE6A-696D-4930-A7F0-EEAC89FE5E4D}"/>
-    <hyperlink ref="D29" r:id="rId24" xr:uid="{484C9603-5306-41D1-80A8-846D2759712C}"/>
-    <hyperlink ref="D28" r:id="rId25" display="https://katalog.we-online.de/em/datasheet/6130xx11121.pdf" xr:uid="{A4FD35A8-382F-4C86-9E06-5143FCB65F6D}"/>
-    <hyperlink ref="D38" r:id="rId26" display="http://www.ti.com/lit/ds/symlink/sn74hc595.pdf" xr:uid="{06113F77-C44E-4230-9895-41937B419CB7}"/>
-    <hyperlink ref="D40" r:id="rId27" display="http://www.vishay.com/docs/45171/kseries.pdf" xr:uid="{E5EF8C94-8FF3-4CA8-9B9E-87F6E9DB4092}"/>
-    <hyperlink ref="D39" r:id="rId28" xr:uid="{FC8D83A5-9C1A-4F8F-B14D-32D28D960C5F}"/>
-    <hyperlink ref="D42" r:id="rId29" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643814&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{E3A30A47-2BA3-4731-BBCD-B356DAFFADB8}"/>
-    <hyperlink ref="D43" r:id="rId30" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643075&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{8B16C1D1-DD20-434B-8323-AF5F2EDA724D}"/>
-    <hyperlink ref="D27" r:id="rId31" display="https://www.nidec-copal-electronics.com/e/catalog/trimmer/sm-42&amp;sm-43.pdf" xr:uid="{D60C1852-FE22-4206-B3C9-619A0EF72358}"/>
-    <hyperlink ref="D34" r:id="rId32" display="https://www.onsemi.com/pub/Collateral/PZT3904-D.pdf" xr:uid="{9523DBC2-EEE9-478C-ADAF-70DD47AC3E92}"/>
-    <hyperlink ref="D33" r:id="rId33" display="https://cdn.harwin.com/pdfs/M20-976.pdf" xr:uid="{34521EE4-CF7E-4C34-8BD1-8EFE6C6D15C2}"/>
-    <hyperlink ref="D32" r:id="rId34" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf" xr:uid="{B2D11C3C-0234-4231-ABA9-DAD532102B77}"/>
-    <hyperlink ref="D31" r:id="rId35" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf" xr:uid="{31B22529-345B-4FCB-8E6C-90977DD52DC7}"/>
-    <hyperlink ref="D30" r:id="rId36" display="https://cdn-shop.adafruit.com/product-files/181/p181.pdf" xr:uid="{7C648116-FDBE-4031-A56C-760A7B342F84}"/>
-    <hyperlink ref="D46" r:id="rId37" display="https://www.onsemi.com/pub/Collateral/PZT3904-D.pdf" xr:uid="{522BDBC1-95E2-4FE2-8E78-6926BF8F4AB5}"/>
-    <hyperlink ref="D44" r:id="rId38" display="https://www.seielect.com/Catalog/SEI-CF_CFM.pdf" xr:uid="{B853B86B-D505-494B-B1DA-2C9007C74A6B}"/>
-    <hyperlink ref="D45" r:id="rId39" display="https://www.seielect.com/Catalog/SEI-CF_CFM.pdf" xr:uid="{D72F90B3-B09E-4086-903B-D01CF76A5649}"/>
-    <hyperlink ref="D26" r:id="rId40" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf" xr:uid="{5A507544-7488-44B1-950F-17D15B2ACC05}"/>
-    <hyperlink ref="D47" r:id="rId41" display="https://www.bourns.com/docs/Product-Datasheets/3362.pdf" xr:uid="{5D4ECA67-0725-426A-95DE-6F19F5E62251}"/>
-    <hyperlink ref="D48" r:id="rId42" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=881545&amp;DocType=Customer+Drawing&amp;DocLang=English" xr:uid="{51B0B09B-6DDC-4FE8-A981-9C937067B97E}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="D13" r:id="rId11"/>
+    <hyperlink ref="D16" r:id="rId12"/>
+    <hyperlink ref="D17" r:id="rId13"/>
+    <hyperlink ref="D18" r:id="rId14"/>
+    <hyperlink ref="D19" r:id="rId15"/>
+    <hyperlink ref="D20" r:id="rId16"/>
+    <hyperlink ref="D14" r:id="rId17"/>
+    <hyperlink ref="D15" r:id="rId18"/>
+    <hyperlink ref="D21" r:id="rId19"/>
+    <hyperlink ref="D22" r:id="rId20"/>
+    <hyperlink ref="D23" r:id="rId21"/>
+    <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D25" r:id="rId23"/>
+    <hyperlink ref="D29" r:id="rId24"/>
+    <hyperlink ref="D28" r:id="rId25" display="https://katalog.we-online.de/em/datasheet/6130xx11121.pdf"/>
+    <hyperlink ref="D38" r:id="rId26" display="http://www.ti.com/lit/ds/symlink/sn74hc595.pdf"/>
+    <hyperlink ref="D40" r:id="rId27" display="http://www.vishay.com/docs/45171/kseries.pdf"/>
+    <hyperlink ref="D39" r:id="rId28"/>
+    <hyperlink ref="D42" r:id="rId29" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643814&amp;DocType=Customer+Drawing&amp;DocLang=English"/>
+    <hyperlink ref="D43" r:id="rId30" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=643075&amp;DocType=Customer+Drawing&amp;DocLang=English"/>
+    <hyperlink ref="D27" r:id="rId31" display="https://www.nidec-copal-electronics.com/e/catalog/trimmer/sm-42&amp;sm-43.pdf"/>
+    <hyperlink ref="D34" r:id="rId32" display="https://www.onsemi.com/pub/Collateral/PZT3904-D.pdf"/>
+    <hyperlink ref="D33" r:id="rId33" display="https://cdn.harwin.com/pdfs/M20-976.pdf"/>
+    <hyperlink ref="D32" r:id="rId34" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf"/>
+    <hyperlink ref="D31" r:id="rId35" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf"/>
+    <hyperlink ref="D30" r:id="rId36" display="https://cdn-shop.adafruit.com/product-files/181/p181.pdf"/>
+    <hyperlink ref="D46" r:id="rId37" display="https://www.onsemi.com/pub/Collateral/PZT3904-D.pdf"/>
+    <hyperlink ref="D44" r:id="rId38" display="https://www.seielect.com/Catalog/SEI-CF_CFM.pdf"/>
+    <hyperlink ref="D45" r:id="rId39" display="https://www.seielect.com/Catalog/SEI-CF_CFM.pdf"/>
+    <hyperlink ref="D26" r:id="rId40" display="http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf"/>
+    <hyperlink ref="D47" r:id="rId41" display="https://www.bourns.com/docs/Product-Datasheets/3362.pdf"/>
+    <hyperlink ref="D48" r:id="rId42" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=881545&amp;DocType=Customer+Drawing&amp;DocLang=English"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId43"/>

</xml_diff>